<commit_message>
Add Stat Grad B1
</commit_message>
<xml_diff>
--- a/Others_Solutions/Ст. Инф. 22.10.2020.(Ф.)/09/9.xlsx
+++ b/Others_Solutions/Ст. Инф. 22.10.2020.(Ф.)/09/9.xlsx
@@ -1,45 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\К-ЕГЭ- 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hem12\Documents\Документы Миша\Школьные предметы\ЕГЭ информатика\Solutions\PrepareForEGE_MishaPolykovsky\Others_Solutions\Ст. Инф. 22.10.2020.(Ф.)\09\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29AF2F1-880D-4190-83A6-EA51799BA155}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист3" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -48,8 +39,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,6 +61,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -72,19 +76,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,16 +402,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -478,7 +485,7 @@
         <v>0.95833333333333304</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43191</v>
       </c>
@@ -554,8 +561,16 @@
       <c r="Y2" s="4">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2">
+        <f>IF(MAX(B2:Y2) - MIN(B2:Y2) &gt; 17, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="6">
+        <f>SUM(Z:Z)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43192</v>
       </c>
@@ -631,8 +646,12 @@
       <c r="Y3" s="4">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z66" si="0">IF(MAX(B3:Y3) - MIN(B3:Y3) &gt; 17, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43193</v>
       </c>
@@ -708,8 +727,12 @@
       <c r="Y4" s="4">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43194</v>
       </c>
@@ -785,8 +808,12 @@
       <c r="Y5" s="4">
         <v>15.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43195</v>
       </c>
@@ -862,8 +889,12 @@
       <c r="Y6" s="4">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43196</v>
       </c>
@@ -939,8 +970,12 @@
       <c r="Y7" s="4">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43197</v>
       </c>
@@ -1016,8 +1051,12 @@
       <c r="Y8" s="4">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43198</v>
       </c>
@@ -1093,8 +1132,12 @@
       <c r="Y9" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43199</v>
       </c>
@@ -1170,8 +1213,12 @@
       <c r="Y10" s="4">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43200</v>
       </c>
@@ -1247,8 +1294,12 @@
       <c r="Y11" s="4">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43201</v>
       </c>
@@ -1324,8 +1375,12 @@
       <c r="Y12" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43202</v>
       </c>
@@ -1401,8 +1456,12 @@
       <c r="Y13" s="4">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43203</v>
       </c>
@@ -1478,8 +1537,12 @@
       <c r="Y14" s="4">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43204</v>
       </c>
@@ -1555,8 +1618,12 @@
       <c r="Y15" s="4">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43205</v>
       </c>
@@ -1632,8 +1699,12 @@
       <c r="Y16" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43206</v>
       </c>
@@ -1709,8 +1780,12 @@
       <c r="Y17" s="4">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43207</v>
       </c>
@@ -1786,8 +1861,12 @@
       <c r="Y18" s="4">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43208</v>
       </c>
@@ -1863,8 +1942,12 @@
       <c r="Y19" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43209</v>
       </c>
@@ -1940,8 +2023,12 @@
       <c r="Y20" s="4">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43210</v>
       </c>
@@ -2017,8 +2104,12 @@
       <c r="Y21" s="4">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43211</v>
       </c>
@@ -2094,8 +2185,12 @@
       <c r="Y22" s="4">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>43212</v>
       </c>
@@ -2171,8 +2266,12 @@
       <c r="Y23" s="4">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43213</v>
       </c>
@@ -2248,8 +2347,12 @@
       <c r="Y24" s="4">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>43214</v>
       </c>
@@ -2325,8 +2428,12 @@
       <c r="Y25" s="4">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43215</v>
       </c>
@@ -2402,8 +2509,12 @@
       <c r="Y26" s="4">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>43216</v>
       </c>
@@ -2479,8 +2590,12 @@
       <c r="Y27" s="4">
         <v>13.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43217</v>
       </c>
@@ -2556,8 +2671,12 @@
       <c r="Y28" s="4">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43218</v>
       </c>
@@ -2633,8 +2752,12 @@
       <c r="Y29" s="4">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43219</v>
       </c>
@@ -2710,8 +2833,12 @@
       <c r="Y30" s="4">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43220</v>
       </c>
@@ -2787,8 +2914,12 @@
       <c r="Y31" s="4">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43221</v>
       </c>
@@ -2864,8 +2995,12 @@
       <c r="Y32" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43222</v>
       </c>
@@ -2941,8 +3076,12 @@
       <c r="Y33" s="4">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43223</v>
       </c>
@@ -3018,8 +3157,12 @@
       <c r="Y34" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43224</v>
       </c>
@@ -3095,8 +3238,12 @@
       <c r="Y35" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43225</v>
       </c>
@@ -3172,8 +3319,12 @@
       <c r="Y36" s="4">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43226</v>
       </c>
@@ -3249,8 +3400,12 @@
       <c r="Y37" s="4">
         <v>21.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43227</v>
       </c>
@@ -3326,8 +3481,12 @@
       <c r="Y38" s="4">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43228</v>
       </c>
@@ -3403,8 +3562,12 @@
       <c r="Y39" s="4">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43229</v>
       </c>
@@ -3480,8 +3643,12 @@
       <c r="Y40" s="4">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43230</v>
       </c>
@@ -3557,8 +3724,12 @@
       <c r="Y41" s="4">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43231</v>
       </c>
@@ -3634,8 +3805,12 @@
       <c r="Y42" s="4">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43232</v>
       </c>
@@ -3711,8 +3886,12 @@
       <c r="Y43" s="4">
         <v>21.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43233</v>
       </c>
@@ -3788,8 +3967,12 @@
       <c r="Y44" s="4">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43234</v>
       </c>
@@ -3865,8 +4048,12 @@
       <c r="Y45" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43235</v>
       </c>
@@ -3942,8 +4129,12 @@
       <c r="Y46" s="4">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43236</v>
       </c>
@@ -4019,8 +4210,12 @@
       <c r="Y47" s="4">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43237</v>
       </c>
@@ -4096,8 +4291,12 @@
       <c r="Y48" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43238</v>
       </c>
@@ -4173,8 +4372,12 @@
       <c r="Y49" s="4">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43239</v>
       </c>
@@ -4250,8 +4453,12 @@
       <c r="Y50" s="4">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43240</v>
       </c>
@@ -4327,8 +4534,12 @@
       <c r="Y51" s="4">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43241</v>
       </c>
@@ -4404,8 +4615,12 @@
       <c r="Y52" s="4">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43242</v>
       </c>
@@ -4481,8 +4696,12 @@
       <c r="Y53" s="4">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>43243</v>
       </c>
@@ -4558,8 +4777,12 @@
       <c r="Y54" s="4">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>43244</v>
       </c>
@@ -4635,8 +4858,12 @@
       <c r="Y55" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>43245</v>
       </c>
@@ -4712,8 +4939,12 @@
       <c r="Y56" s="4">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>43246</v>
       </c>
@@ -4789,8 +5020,12 @@
       <c r="Y57" s="4">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>43247</v>
       </c>
@@ -4866,8 +5101,12 @@
       <c r="Y58" s="4">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>43248</v>
       </c>
@@ -4943,8 +5182,12 @@
       <c r="Y59" s="4">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>43249</v>
       </c>
@@ -5020,8 +5263,12 @@
       <c r="Y60" s="4">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>43250</v>
       </c>
@@ -5097,8 +5344,12 @@
       <c r="Y61" s="4">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>43251</v>
       </c>
@@ -5174,8 +5425,12 @@
       <c r="Y62" s="4">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>43252</v>
       </c>
@@ -5251,8 +5506,12 @@
       <c r="Y63" s="4">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>43253</v>
       </c>
@@ -5328,8 +5587,12 @@
       <c r="Y64" s="4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>43254</v>
       </c>
@@ -5405,8 +5668,12 @@
       <c r="Y65" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>43255</v>
       </c>
@@ -5482,8 +5749,12 @@
       <c r="Y66" s="4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>43256</v>
       </c>
@@ -5559,8 +5830,12 @@
       <c r="Y67" s="4">
         <v>28.3</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z67">
+        <f t="shared" ref="Z67:Z92" si="1">IF(MAX(B67:Y67) - MIN(B67:Y67) &gt; 17, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>43257</v>
       </c>
@@ -5636,8 +5911,12 @@
       <c r="Y68" s="4">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>43258</v>
       </c>
@@ -5713,8 +5992,12 @@
       <c r="Y69" s="4">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>43259</v>
       </c>
@@ -5790,8 +6073,12 @@
       <c r="Y70" s="4">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>43260</v>
       </c>
@@ -5867,8 +6154,12 @@
       <c r="Y71" s="4">
         <v>27.7</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>43261</v>
       </c>
@@ -5944,8 +6235,12 @@
       <c r="Y72" s="4">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>43262</v>
       </c>
@@ -6021,8 +6316,12 @@
       <c r="Y73" s="4">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>43263</v>
       </c>
@@ -6098,8 +6397,12 @@
       <c r="Y74" s="4">
         <v>28.8</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z74">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>43264</v>
       </c>
@@ -6175,8 +6478,12 @@
       <c r="Y75" s="4">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>43265</v>
       </c>
@@ -6252,8 +6559,12 @@
       <c r="Y76" s="4">
         <v>28.7</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>43266</v>
       </c>
@@ -6329,8 +6640,12 @@
       <c r="Y77" s="4">
         <v>25.3</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z77">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>43267</v>
       </c>
@@ -6406,8 +6721,12 @@
       <c r="Y78" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>43268</v>
       </c>
@@ -6483,8 +6802,12 @@
       <c r="Y79" s="4">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z79">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>43269</v>
       </c>
@@ -6560,8 +6883,12 @@
       <c r="Y80" s="4">
         <v>26.2</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>43270</v>
       </c>
@@ -6637,8 +6964,12 @@
       <c r="Y81" s="4">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z81">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>43271</v>
       </c>
@@ -6714,8 +7045,12 @@
       <c r="Y82" s="4">
         <v>27.2</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z82">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>43272</v>
       </c>
@@ -6791,8 +7126,12 @@
       <c r="Y83" s="4">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z83">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>43273</v>
       </c>
@@ -6868,8 +7207,12 @@
       <c r="Y84" s="4">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>43274</v>
       </c>
@@ -6945,8 +7288,12 @@
       <c r="Y85" s="4">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z85">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>43275</v>
       </c>
@@ -7022,8 +7369,12 @@
       <c r="Y86" s="4">
         <v>25.1</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z86">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>43276</v>
       </c>
@@ -7099,8 +7450,12 @@
       <c r="Y87" s="4">
         <v>28.3</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z87">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>43277</v>
       </c>
@@ -7176,8 +7531,12 @@
       <c r="Y88" s="4">
         <v>28.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z88">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>43278</v>
       </c>
@@ -7253,8 +7612,12 @@
       <c r="Y89" s="4">
         <v>26.4</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>43279</v>
       </c>
@@ -7330,8 +7693,12 @@
       <c r="Y90" s="4">
         <v>27.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z90">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>43280</v>
       </c>
@@ -7407,8 +7774,12 @@
       <c r="Y91" s="4">
         <v>27.7</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z91">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>43281</v>
       </c>
@@ -7484,11 +7855,15 @@
       <c r="Y92" s="4">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z92">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C96" s="3"/>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>